<commit_message>
Trabalho com os métodos de ordenação
</commit_message>
<xml_diff>
--- a/relatorio.xlsx
+++ b/relatorio.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Documents\Projetos-GIT\puc-lab03-atv1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="12_ncr:500000_{91C9EE36-1462-417E-9D30-89C61C7CE0BB}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31"/>
+  <xr:revisionPtr documentId="10_ncr:8100000_{3C7AB414-CD6B-467C-8E97-2E111CD1368D}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32"/>
   <bookViews>
     <workbookView windowHeight="7650" windowWidth="20490" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
   <si>
     <t>Método de Ordenação</t>
   </si>
@@ -60,40 +60,31 @@
     <t>Tamanho: 10.000.000</t>
   </si>
   <si>
-    <t>22/04/2018 12:09:02</t>
-  </si>
-  <si>
     <t>Tamanho: 1.000.000</t>
   </si>
   <si>
-    <t>22/04/2018 12:10:00</t>
-  </si>
-  <si>
-    <t>22/04/2018 12:10:01</t>
-  </si>
-  <si>
-    <t>22/04/2018 12:10:02</t>
-  </si>
-  <si>
-    <t>22/04/2018 12:10:04</t>
-  </si>
-  <si>
-    <t>22/04/2018 12:10:05</t>
-  </si>
-  <si>
-    <t>22/04/2018 12:11:41</t>
-  </si>
-  <si>
-    <t>22/04/2018 12:11:42</t>
-  </si>
-  <si>
-    <t>22/04/2018 12:11:43</t>
-  </si>
-  <si>
-    <t>22/04/2018 12:11:44</t>
-  </si>
-  <si>
-    <t>22/04/2018 12:11:46</t>
+    <t>Selection</t>
+  </si>
+  <si>
+    <t>Shell</t>
+  </si>
+  <si>
+    <t>Heap</t>
+  </si>
+  <si>
+    <t>12/05/2018 23:27:45</t>
+  </si>
+  <si>
+    <t>Bubble</t>
+  </si>
+  <si>
+    <t>12/05/2018 23:31:42</t>
+  </si>
+  <si>
+    <t>12/05/2018 23:31:43</t>
+  </si>
+  <si>
+    <t>12/05/2018 23:31:44</t>
   </si>
 </sst>
 </file>
@@ -178,8 +169,8 @@
     <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
@@ -187,8 +178,8 @@
     <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="center"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -473,7 +464,7 @@
   <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +472,7 @@
     <col min="1" max="1" bestFit="true" customWidth="true" width="31.42578125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="12" width="21.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="9" width="21.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row ht="18" r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -489,7 +480,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="8"/>
@@ -513,188 +504,274 @@
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="D4" s="12" t="n">
-        <v>20.0</v>
+        <v>10.0</v>
+      </c>
+      <c r="D4" s="9">
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="12">
         <v>349</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>22.0</v>
-      </c>
-      <c r="D5" s="12" t="n">
-        <v>37.0</v>
+        <v>28.0</v>
+      </c>
+      <c r="D5" s="9">
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="12">
         <v>396</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="D6" s="12" t="n">
-        <v>38.0</v>
+        <v>11.0</v>
+      </c>
+      <c r="D6" s="9">
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>97.0</v>
-      </c>
-      <c r="D7" s="12" t="n">
-        <v>422.0</v>
+        <v>139.0</v>
+      </c>
+      <c r="D7" s="9">
+        <v>380</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="5" t="n">
-        <v>94.0</v>
-      </c>
-      <c r="D8" s="12" t="n">
-        <v>407.0</v>
+        <v>164.0</v>
+      </c>
+      <c r="D8" s="9">
+        <v>400</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="5" t="n">
-        <v>49.0</v>
-      </c>
-      <c r="D9" s="12" t="n">
-        <v>406.0</v>
+        <v>71.0</v>
+      </c>
+      <c r="D9" s="9">
+        <v>393</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="5" t="n">
-        <v>77.0</v>
-      </c>
-      <c r="D10" s="12" t="n">
-        <v>296.0</v>
+        <v>87.0</v>
+      </c>
+      <c r="D10" s="9">
+        <v>302</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="5" t="n">
-        <v>49.0</v>
-      </c>
-      <c r="D11" s="12" t="n">
-        <v>301.0</v>
+        <v>65.0</v>
+      </c>
+      <c r="D11" s="9">
+        <v>308</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="5" t="n">
-        <v>53.0</v>
-      </c>
-      <c r="D12" s="12" t="n">
-        <v>306.0</v>
+        <v>80.0</v>
+      </c>
+      <c r="D12" s="9">
+        <v>300</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="5"/>
+      <c r="A13" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="9"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="5"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="9"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="5"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="9"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="9" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="D16" s="9">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="9" t="n">
+        <v>91.0</v>
+      </c>
+      <c r="D17" s="9">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="9" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="D18" s="9">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="9" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="D19" s="9">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="9" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="D20" s="9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="9" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="D21" s="9">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="9"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="9"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="9"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C30" s="4"/>
     </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C31" s="4"/>
     </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C32" s="4"/>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
@@ -782,7 +859,11 @@
       <c r="C60" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="10">
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A13:A15"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="A7:A9"/>

</xml_diff>